<commit_message>
integrated new versions of funcs
</commit_message>
<xml_diff>
--- a/input_sheets/VWR testing.xlsx
+++ b/input_sheets/VWR testing.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -575,7 +575,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -623,7 +623,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -683,7 +683,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -695,7 +695,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -743,7 +743,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -755,7 +755,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -767,7 +767,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -815,7 +815,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -863,7 +863,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -875,7 +875,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -899,7 +899,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -923,7 +923,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -959,7 +959,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -983,7 +983,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -995,7 +995,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1103,7 +1103,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1475,7 +1475,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1631,7 +1631,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1763,7 +1763,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -1989,6 +1989,7 @@
           <t>03AFC15605</t>
         </is>
       </c>
+      <c r="B129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="2" t="inlineStr">
@@ -1996,11 +1997,7 @@
           <t>03SB00705</t>
         </is>
       </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>Chemicals</t>
-        </is>
-      </c>
+      <c r="B130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" s="2" t="inlineStr">
@@ -2008,11 +2005,7 @@
           <t>03SB00710</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>Chemicals</t>
-        </is>
-      </c>
+      <c r="B131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" s="2" t="inlineStr">
@@ -2106,7 +2099,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -2118,7 +2111,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -2128,6 +2121,7 @@
           <t>04822521</t>
         </is>
       </c>
+      <c r="B141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" s="2" t="inlineStr">
@@ -2135,6 +2129,7 @@
           <t>07WS1075</t>
         </is>
       </c>
+      <c r="B142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" s="2" t="inlineStr">
@@ -2144,7 +2139,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies, Protein, Peptides, Enzymes, Chemicals</t>
         </is>
       </c>
     </row>
@@ -2156,7 +2151,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2168,7 +2163,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies, Protein, Peptides, Enzymes</t>
         </is>
       </c>
     </row>
@@ -2180,7 +2175,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2192,7 +2187,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies, Protein, Peptides, Enzymes</t>
         </is>
       </c>
     </row>
@@ -2204,7 +2199,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2216,7 +2211,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2228,7 +2223,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2240,7 +2235,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2252,7 +2247,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2264,7 +2259,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2276,7 +2271,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2288,7 +2283,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2300,7 +2295,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies, Protein, Peptides, Enzymes</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2307,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies</t>
         </is>
       </c>
     </row>
@@ -2324,7 +2319,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies, Chemicals</t>
         </is>
       </c>
     </row>
@@ -2336,7 +2331,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Antibody</t>
+          <t>Antibodies, Chemicals</t>
         </is>
       </c>
     </row>
@@ -2456,7 +2451,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Cell Culture Media</t>
+          <t>Cell Culture Media, Chemicals</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2535,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Protein, Peptides, Enzymes</t>
+          <t>Cell Culture Media</t>
         </is>
       </c>
     </row>
@@ -2550,6 +2545,11 @@
           <t>113070044</t>
         </is>
       </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Cell Culture Media</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="2" t="inlineStr">
@@ -2557,6 +2557,11 @@
           <t>113100132</t>
         </is>
       </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Cell Culture Media</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="2" t="inlineStr">
@@ -2564,6 +2569,11 @@
           <t>113100142</t>
         </is>
       </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Cell Culture Media</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="2" t="inlineStr">
@@ -2571,6 +2581,11 @@
           <t>113301100</t>
         </is>
       </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Cell Culture Media</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="2" t="inlineStr">
@@ -2578,6 +2593,11 @@
           <t>114026932</t>
         </is>
       </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Cell Culture Media</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="inlineStr">
@@ -2585,6 +2605,11 @@
           <t>114029622</t>
         </is>
       </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Cell Culture Media</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="2" t="inlineStr">
@@ -2592,6 +2617,11 @@
           <t>114420122</t>
         </is>
       </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Cell Culture Media</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="2" t="inlineStr">
@@ -2599,6 +2629,7 @@
           <t>116002554</t>
         </is>
       </c>
+      <c r="B184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" s="2" t="inlineStr">
@@ -2606,6 +2637,7 @@
           <t>116550900</t>
         </is>
       </c>
+      <c r="B185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" s="2" t="inlineStr">
@@ -2613,6 +2645,7 @@
           <t>116914801</t>
         </is>
       </c>
+      <c r="B186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" s="2" t="inlineStr">
@@ -2620,6 +2653,7 @@
           <t>116950000</t>
         </is>
       </c>
+      <c r="B187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" s="2" t="inlineStr">
@@ -2627,6 +2661,7 @@
           <t>116954100</t>
         </is>
       </c>
+      <c r="B188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" s="2" t="inlineStr">
@@ -2634,6 +2669,7 @@
           <t>116990100</t>
         </is>
       </c>
+      <c r="B189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" s="2" t="inlineStr">
@@ -2641,6 +2677,11 @@
           <t>11AGAH0100</t>
         </is>
       </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="2" t="inlineStr">
@@ -2648,6 +2689,11 @@
           <t>11BIAC2902</t>
         </is>
       </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="2" t="inlineStr">
@@ -2655,11 +2701,7 @@
           <t>11EPHSP025</t>
         </is>
       </c>
-      <c r="B192" t="inlineStr">
-        <is>
-          <t>Protein, Peptides, Enzymes</t>
-        </is>
-      </c>
+      <c r="B192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" s="2" t="inlineStr">
@@ -2667,6 +2709,11 @@
           <t>11FORMD002</t>
         </is>
       </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="2" t="inlineStr">
@@ -2674,6 +2721,7 @@
           <t>11NTATP100</t>
         </is>
       </c>
+      <c r="B194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" s="2" t="inlineStr">
@@ -2681,6 +2729,7 @@
           <t>11NTCTP100</t>
         </is>
       </c>
+      <c r="B195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" s="2" t="inlineStr">
@@ -2688,6 +2737,7 @@
           <t>11NTGTP100</t>
         </is>
       </c>
+      <c r="B196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" s="2" t="inlineStr">
@@ -2695,6 +2745,7 @@
           <t>11NTTTP100</t>
         </is>
       </c>
+      <c r="B197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" s="2" t="inlineStr">
@@ -2702,11 +2753,7 @@
           <t>11RIST1373</t>
         </is>
       </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>Protein, Peptides, Enzymes</t>
-        </is>
-      </c>
+      <c r="B198" t="inlineStr"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>